<commit_message>
finished student and teacher role
</commit_message>
<xml_diff>
--- a/excel/grade_12 វិទ្យាសាស្រ្ត.xlsx
+++ b/excel/grade_12 វិទ្យាសាស្រ្ត.xlsx
@@ -5,10 +5,10 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\Project\school_cms_folder\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\Project\school_cms_folder\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15CB6E42-54CD-4051-90C3-B51C391F3A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F7A4AFB2-5159-4F4F-A757-2E28D11E479F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EBC9FFE7-F7AF-453A-AB6D-2E0E8F98E0C7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="281" uniqueCount="190">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="438" uniqueCount="199">
   <si>
     <t>full_name_kh</t>
   </si>
@@ -595,6 +595,33 @@
   </si>
   <si>
     <t>S2026400</t>
+  </si>
+  <si>
+    <t>father_job</t>
+  </si>
+  <si>
+    <t>Mother_job</t>
+  </si>
+  <si>
+    <t>father_phone</t>
+  </si>
+  <si>
+    <t>mother_phone</t>
+  </si>
+  <si>
+    <t>not</t>
+  </si>
+  <si>
+    <t>class_id</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>academic_year</t>
+  </si>
+  <si>
+    <t>2024-2025</t>
   </si>
 </sst>
 </file>
@@ -1456,10 +1483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D4ED42-DECB-4864-A548-78E7BE524A82}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1468,7 +1495,7 @@
     <col min="5" max="5" width="68.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1493,17 +1520,38 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>190</v>
+      </c>
+      <c r="K1" t="s">
+        <v>191</v>
+      </c>
+      <c r="L1" t="s">
+        <v>192</v>
+      </c>
+      <c r="M1" t="s">
+        <v>193</v>
+      </c>
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
+      <c r="Q1" t="s">
+        <v>195</v>
+      </c>
+      <c r="R1" t="s">
+        <v>196</v>
+      </c>
+      <c r="S1" t="s">
+        <v>197</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1528,17 +1576,38 @@
       <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
+        <v>194</v>
+      </c>
+      <c r="K2" t="s">
+        <v>194</v>
+      </c>
+      <c r="L2" t="s">
+        <v>194</v>
+      </c>
+      <c r="M2" t="s">
+        <v>194</v>
+      </c>
+      <c r="N2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
+      <c r="O2" t="s">
         <v>18</v>
       </c>
-      <c r="K2">
+      <c r="P2">
         <v>12</v>
       </c>
+      <c r="Q2">
+        <v>8</v>
+      </c>
+      <c r="R2">
+        <v>11</v>
+      </c>
+      <c r="S2" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1563,17 +1632,38 @@
       <c r="H3" t="s">
         <v>25</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
+        <v>194</v>
+      </c>
+      <c r="K3" t="s">
+        <v>194</v>
+      </c>
+      <c r="L3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M3" t="s">
+        <v>194</v>
+      </c>
+      <c r="N3" t="s">
         <v>26</v>
       </c>
-      <c r="J3" t="s">
+      <c r="O3" t="s">
         <v>18</v>
       </c>
-      <c r="K3">
+      <c r="P3">
         <v>12</v>
       </c>
+      <c r="Q3">
+        <v>8</v>
+      </c>
+      <c r="R3">
+        <v>11</v>
+      </c>
+      <c r="S3" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1598,17 +1688,38 @@
       <c r="H4" t="s">
         <v>32</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
+        <v>194</v>
+      </c>
+      <c r="K4" t="s">
+        <v>194</v>
+      </c>
+      <c r="L4" t="s">
+        <v>194</v>
+      </c>
+      <c r="M4" t="s">
+        <v>194</v>
+      </c>
+      <c r="N4" t="s">
         <v>33</v>
       </c>
-      <c r="J4" t="s">
+      <c r="O4" t="s">
         <v>18</v>
       </c>
-      <c r="K4">
+      <c r="P4">
         <v>12</v>
       </c>
+      <c r="Q4">
+        <v>8</v>
+      </c>
+      <c r="R4">
+        <v>11</v>
+      </c>
+      <c r="S4" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1633,17 +1744,38 @@
       <c r="H5" t="s">
         <v>39</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
+        <v>194</v>
+      </c>
+      <c r="K5" t="s">
+        <v>194</v>
+      </c>
+      <c r="L5" t="s">
+        <v>194</v>
+      </c>
+      <c r="M5" t="s">
+        <v>194</v>
+      </c>
+      <c r="N5" t="s">
         <v>40</v>
       </c>
-      <c r="J5" t="s">
+      <c r="O5" t="s">
         <v>18</v>
       </c>
-      <c r="K5">
+      <c r="P5">
         <v>12</v>
       </c>
+      <c r="Q5">
+        <v>8</v>
+      </c>
+      <c r="R5">
+        <v>11</v>
+      </c>
+      <c r="S5" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1668,17 +1800,38 @@
       <c r="H6" t="s">
         <v>45</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
+        <v>194</v>
+      </c>
+      <c r="K6" t="s">
+        <v>194</v>
+      </c>
+      <c r="L6" t="s">
+        <v>194</v>
+      </c>
+      <c r="M6" t="s">
+        <v>194</v>
+      </c>
+      <c r="N6" t="s">
         <v>46</v>
       </c>
-      <c r="J6" t="s">
+      <c r="O6" t="s">
         <v>18</v>
       </c>
-      <c r="K6">
+      <c r="P6">
         <v>12</v>
       </c>
+      <c r="Q6">
+        <v>8</v>
+      </c>
+      <c r="R6">
+        <v>11</v>
+      </c>
+      <c r="S6" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -1703,17 +1856,38 @@
       <c r="H7" t="s">
         <v>52</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
+        <v>194</v>
+      </c>
+      <c r="K7" t="s">
+        <v>194</v>
+      </c>
+      <c r="L7" t="s">
+        <v>194</v>
+      </c>
+      <c r="M7" t="s">
+        <v>194</v>
+      </c>
+      <c r="N7" t="s">
         <v>53</v>
       </c>
-      <c r="J7" t="s">
+      <c r="O7" t="s">
         <v>18</v>
       </c>
-      <c r="K7">
+      <c r="P7">
         <v>12</v>
       </c>
+      <c r="Q7">
+        <v>8</v>
+      </c>
+      <c r="R7">
+        <v>11</v>
+      </c>
+      <c r="S7" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -1738,17 +1912,38 @@
       <c r="H8" t="s">
         <v>58</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
+        <v>194</v>
+      </c>
+      <c r="K8" t="s">
+        <v>194</v>
+      </c>
+      <c r="L8" t="s">
+        <v>194</v>
+      </c>
+      <c r="M8" t="s">
+        <v>194</v>
+      </c>
+      <c r="N8" t="s">
         <v>59</v>
       </c>
-      <c r="J8" t="s">
+      <c r="O8" t="s">
         <v>18</v>
       </c>
-      <c r="K8">
+      <c r="P8">
         <v>12</v>
       </c>
+      <c r="Q8">
+        <v>8</v>
+      </c>
+      <c r="R8">
+        <v>11</v>
+      </c>
+      <c r="S8" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -1773,17 +1968,38 @@
       <c r="H9" t="s">
         <v>64</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
+        <v>194</v>
+      </c>
+      <c r="K9" t="s">
+        <v>194</v>
+      </c>
+      <c r="L9" t="s">
+        <v>194</v>
+      </c>
+      <c r="M9" t="s">
+        <v>194</v>
+      </c>
+      <c r="N9" t="s">
         <v>65</v>
       </c>
-      <c r="J9" t="s">
+      <c r="O9" t="s">
         <v>18</v>
       </c>
-      <c r="K9">
+      <c r="P9">
         <v>12</v>
       </c>
+      <c r="Q9">
+        <v>8</v>
+      </c>
+      <c r="R9">
+        <v>11</v>
+      </c>
+      <c r="S9" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -1808,17 +2024,38 @@
       <c r="H10" t="s">
         <v>70</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
+        <v>194</v>
+      </c>
+      <c r="K10" t="s">
+        <v>194</v>
+      </c>
+      <c r="L10" t="s">
+        <v>194</v>
+      </c>
+      <c r="M10" t="s">
+        <v>194</v>
+      </c>
+      <c r="N10" t="s">
         <v>71</v>
       </c>
-      <c r="J10" t="s">
+      <c r="O10" t="s">
         <v>18</v>
       </c>
-      <c r="K10">
+      <c r="P10">
         <v>12</v>
       </c>
+      <c r="Q10">
+        <v>8</v>
+      </c>
+      <c r="R10">
+        <v>11</v>
+      </c>
+      <c r="S10" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1843,17 +2080,38 @@
       <c r="H11" t="s">
         <v>77</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
+        <v>194</v>
+      </c>
+      <c r="K11" t="s">
+        <v>194</v>
+      </c>
+      <c r="L11" t="s">
+        <v>194</v>
+      </c>
+      <c r="M11" t="s">
+        <v>194</v>
+      </c>
+      <c r="N11" t="s">
         <v>78</v>
       </c>
-      <c r="J11" t="s">
+      <c r="O11" t="s">
         <v>18</v>
       </c>
-      <c r="K11">
+      <c r="P11">
         <v>12</v>
       </c>
+      <c r="Q11">
+        <v>8</v>
+      </c>
+      <c r="R11">
+        <v>11</v>
+      </c>
+      <c r="S11" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>79</v>
       </c>
@@ -1878,17 +2136,38 @@
       <c r="H12" t="s">
         <v>83</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
+        <v>194</v>
+      </c>
+      <c r="K12" t="s">
+        <v>194</v>
+      </c>
+      <c r="L12" t="s">
+        <v>194</v>
+      </c>
+      <c r="M12" t="s">
+        <v>194</v>
+      </c>
+      <c r="N12" t="s">
         <v>84</v>
       </c>
-      <c r="J12" t="s">
+      <c r="O12" t="s">
         <v>18</v>
       </c>
-      <c r="K12">
+      <c r="P12">
         <v>12</v>
       </c>
+      <c r="Q12">
+        <v>8</v>
+      </c>
+      <c r="R12">
+        <v>11</v>
+      </c>
+      <c r="S12" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>85</v>
       </c>
@@ -1913,17 +2192,38 @@
       <c r="H13" t="s">
         <v>90</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
+        <v>194</v>
+      </c>
+      <c r="K13" t="s">
+        <v>194</v>
+      </c>
+      <c r="L13" t="s">
+        <v>194</v>
+      </c>
+      <c r="M13" t="s">
+        <v>194</v>
+      </c>
+      <c r="N13" t="s">
         <v>91</v>
       </c>
-      <c r="J13" t="s">
+      <c r="O13" t="s">
         <v>18</v>
       </c>
-      <c r="K13">
+      <c r="P13">
         <v>12</v>
       </c>
+      <c r="Q13">
+        <v>8</v>
+      </c>
+      <c r="R13">
+        <v>11</v>
+      </c>
+      <c r="S13" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>92</v>
       </c>
@@ -1948,17 +2248,38 @@
       <c r="H14" t="s">
         <v>96</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
+        <v>194</v>
+      </c>
+      <c r="K14" t="s">
+        <v>194</v>
+      </c>
+      <c r="L14" t="s">
+        <v>194</v>
+      </c>
+      <c r="M14" t="s">
+        <v>194</v>
+      </c>
+      <c r="N14" t="s">
         <v>97</v>
       </c>
-      <c r="J14" t="s">
+      <c r="O14" t="s">
         <v>18</v>
       </c>
-      <c r="K14">
+      <c r="P14">
         <v>12</v>
       </c>
+      <c r="Q14">
+        <v>8</v>
+      </c>
+      <c r="R14">
+        <v>11</v>
+      </c>
+      <c r="S14" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>98</v>
       </c>
@@ -1983,17 +2304,38 @@
       <c r="H15" t="s">
         <v>102</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
+        <v>194</v>
+      </c>
+      <c r="K15" t="s">
+        <v>194</v>
+      </c>
+      <c r="L15" t="s">
+        <v>194</v>
+      </c>
+      <c r="M15" t="s">
+        <v>194</v>
+      </c>
+      <c r="N15" t="s">
         <v>103</v>
       </c>
-      <c r="J15" t="s">
+      <c r="O15" t="s">
         <v>18</v>
       </c>
-      <c r="K15">
+      <c r="P15">
         <v>12</v>
       </c>
+      <c r="Q15">
+        <v>8</v>
+      </c>
+      <c r="R15">
+        <v>11</v>
+      </c>
+      <c r="S15" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>104</v>
       </c>
@@ -2018,17 +2360,38 @@
       <c r="H16" t="s">
         <v>108</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
+        <v>194</v>
+      </c>
+      <c r="K16" t="s">
+        <v>194</v>
+      </c>
+      <c r="L16" t="s">
+        <v>194</v>
+      </c>
+      <c r="M16" t="s">
+        <v>194</v>
+      </c>
+      <c r="N16" t="s">
         <v>109</v>
       </c>
-      <c r="J16" t="s">
+      <c r="O16" t="s">
         <v>18</v>
       </c>
-      <c r="K16">
+      <c r="P16">
         <v>12</v>
       </c>
+      <c r="Q16">
+        <v>8</v>
+      </c>
+      <c r="R16">
+        <v>11</v>
+      </c>
+      <c r="S16" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -2053,17 +2416,38 @@
       <c r="H17" t="s">
         <v>114</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
+        <v>194</v>
+      </c>
+      <c r="K17" t="s">
+        <v>194</v>
+      </c>
+      <c r="L17" t="s">
+        <v>194</v>
+      </c>
+      <c r="M17" t="s">
+        <v>194</v>
+      </c>
+      <c r="N17" t="s">
         <v>115</v>
       </c>
-      <c r="J17" t="s">
+      <c r="O17" t="s">
         <v>18</v>
       </c>
-      <c r="K17">
+      <c r="P17">
         <v>12</v>
       </c>
+      <c r="Q17">
+        <v>8</v>
+      </c>
+      <c r="R17">
+        <v>11</v>
+      </c>
+      <c r="S17" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>116</v>
       </c>
@@ -2088,17 +2472,38 @@
       <c r="H18" t="s">
         <v>70</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
+        <v>194</v>
+      </c>
+      <c r="K18" t="s">
+        <v>194</v>
+      </c>
+      <c r="L18" t="s">
+        <v>194</v>
+      </c>
+      <c r="M18" t="s">
+        <v>194</v>
+      </c>
+      <c r="N18" t="s">
         <v>121</v>
       </c>
-      <c r="J18" t="s">
+      <c r="O18" t="s">
         <v>18</v>
       </c>
-      <c r="K18">
+      <c r="P18">
         <v>12</v>
       </c>
+      <c r="Q18">
+        <v>8</v>
+      </c>
+      <c r="R18">
+        <v>11</v>
+      </c>
+      <c r="S18" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>122</v>
       </c>
@@ -2123,17 +2528,38 @@
       <c r="H19" t="s">
         <v>127</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
+        <v>194</v>
+      </c>
+      <c r="K19" t="s">
+        <v>194</v>
+      </c>
+      <c r="L19" t="s">
+        <v>194</v>
+      </c>
+      <c r="M19" t="s">
+        <v>194</v>
+      </c>
+      <c r="N19" t="s">
         <v>128</v>
       </c>
-      <c r="J19" t="s">
+      <c r="O19" t="s">
         <v>18</v>
       </c>
-      <c r="K19">
+      <c r="P19">
         <v>12</v>
       </c>
+      <c r="Q19">
+        <v>8</v>
+      </c>
+      <c r="R19">
+        <v>11</v>
+      </c>
+      <c r="S19" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>129</v>
       </c>
@@ -2158,17 +2584,38 @@
       <c r="H20" t="s">
         <v>133</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
+        <v>194</v>
+      </c>
+      <c r="K20" t="s">
+        <v>194</v>
+      </c>
+      <c r="L20" t="s">
+        <v>194</v>
+      </c>
+      <c r="M20" t="s">
+        <v>194</v>
+      </c>
+      <c r="N20" t="s">
         <v>134</v>
       </c>
-      <c r="J20" t="s">
+      <c r="O20" t="s">
         <v>18</v>
       </c>
-      <c r="K20">
+      <c r="P20">
         <v>12</v>
       </c>
+      <c r="Q20">
+        <v>8</v>
+      </c>
+      <c r="R20">
+        <v>11</v>
+      </c>
+      <c r="S20" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>135</v>
       </c>
@@ -2193,17 +2640,38 @@
       <c r="H21" t="s">
         <v>45</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
+        <v>194</v>
+      </c>
+      <c r="K21" t="s">
+        <v>194</v>
+      </c>
+      <c r="L21" t="s">
+        <v>194</v>
+      </c>
+      <c r="M21" t="s">
+        <v>194</v>
+      </c>
+      <c r="N21" t="s">
         <v>138</v>
       </c>
-      <c r="J21" t="s">
+      <c r="O21" t="s">
         <v>18</v>
       </c>
-      <c r="K21">
+      <c r="P21">
         <v>12</v>
       </c>
+      <c r="Q21">
+        <v>8</v>
+      </c>
+      <c r="R21">
+        <v>11</v>
+      </c>
+      <c r="S21" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>139</v>
       </c>
@@ -2228,17 +2696,38 @@
       <c r="H22" t="s">
         <v>39</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
+        <v>194</v>
+      </c>
+      <c r="K22" t="s">
+        <v>194</v>
+      </c>
+      <c r="L22" t="s">
+        <v>194</v>
+      </c>
+      <c r="M22" t="s">
+        <v>194</v>
+      </c>
+      <c r="N22" t="s">
         <v>142</v>
       </c>
-      <c r="J22" t="s">
+      <c r="O22" t="s">
         <v>18</v>
       </c>
-      <c r="K22">
+      <c r="P22">
         <v>12</v>
       </c>
+      <c r="Q22">
+        <v>8</v>
+      </c>
+      <c r="R22">
+        <v>11</v>
+      </c>
+      <c r="S22" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>143</v>
       </c>
@@ -2263,17 +2752,38 @@
       <c r="H23" t="s">
         <v>16</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
+        <v>194</v>
+      </c>
+      <c r="K23" t="s">
+        <v>194</v>
+      </c>
+      <c r="L23" t="s">
+        <v>194</v>
+      </c>
+      <c r="M23" t="s">
+        <v>194</v>
+      </c>
+      <c r="N23" t="s">
         <v>146</v>
       </c>
-      <c r="J23" t="s">
+      <c r="O23" t="s">
         <v>18</v>
       </c>
-      <c r="K23">
+      <c r="P23">
         <v>12</v>
       </c>
+      <c r="Q23">
+        <v>8</v>
+      </c>
+      <c r="R23">
+        <v>11</v>
+      </c>
+      <c r="S23" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>147</v>
       </c>
@@ -2298,17 +2808,38 @@
       <c r="H24" t="s">
         <v>150</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
+        <v>194</v>
+      </c>
+      <c r="K24" t="s">
+        <v>194</v>
+      </c>
+      <c r="L24" t="s">
+        <v>194</v>
+      </c>
+      <c r="M24" t="s">
+        <v>194</v>
+      </c>
+      <c r="N24" t="s">
         <v>151</v>
       </c>
-      <c r="J24" t="s">
+      <c r="O24" t="s">
         <v>18</v>
       </c>
-      <c r="K24">
+      <c r="P24">
         <v>12</v>
       </c>
+      <c r="Q24">
+        <v>8</v>
+      </c>
+      <c r="R24">
+        <v>11</v>
+      </c>
+      <c r="S24" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>152</v>
       </c>
@@ -2333,17 +2864,38 @@
       <c r="H25" t="s">
         <v>155</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
+        <v>194</v>
+      </c>
+      <c r="K25" t="s">
+        <v>194</v>
+      </c>
+      <c r="L25" t="s">
+        <v>194</v>
+      </c>
+      <c r="M25" t="s">
+        <v>194</v>
+      </c>
+      <c r="N25" t="s">
         <v>156</v>
       </c>
-      <c r="J25" t="s">
+      <c r="O25" t="s">
         <v>18</v>
       </c>
-      <c r="K25">
+      <c r="P25">
         <v>12</v>
       </c>
+      <c r="Q25">
+        <v>8</v>
+      </c>
+      <c r="R25">
+        <v>11</v>
+      </c>
+      <c r="S25" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>157</v>
       </c>
@@ -2368,17 +2920,38 @@
       <c r="H26" t="s">
         <v>114</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
+        <v>194</v>
+      </c>
+      <c r="K26" t="s">
+        <v>194</v>
+      </c>
+      <c r="L26" t="s">
+        <v>194</v>
+      </c>
+      <c r="M26" t="s">
+        <v>194</v>
+      </c>
+      <c r="N26" t="s">
         <v>162</v>
       </c>
-      <c r="J26" t="s">
+      <c r="O26" t="s">
         <v>18</v>
       </c>
-      <c r="K26">
+      <c r="P26">
         <v>12</v>
       </c>
+      <c r="Q26">
+        <v>8</v>
+      </c>
+      <c r="R26">
+        <v>11</v>
+      </c>
+      <c r="S26" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>163</v>
       </c>
@@ -2403,17 +2976,38 @@
       <c r="H27" t="s">
         <v>108</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
+        <v>194</v>
+      </c>
+      <c r="K27" t="s">
+        <v>194</v>
+      </c>
+      <c r="L27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M27" t="s">
+        <v>194</v>
+      </c>
+      <c r="N27" t="s">
         <v>166</v>
       </c>
-      <c r="J27" t="s">
+      <c r="O27" t="s">
         <v>18</v>
       </c>
-      <c r="K27">
+      <c r="P27">
         <v>12</v>
       </c>
+      <c r="Q27">
+        <v>8</v>
+      </c>
+      <c r="R27">
+        <v>11</v>
+      </c>
+      <c r="S27" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>167</v>
       </c>
@@ -2438,17 +3032,38 @@
       <c r="H28" t="s">
         <v>83</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
+        <v>194</v>
+      </c>
+      <c r="K28" t="s">
+        <v>194</v>
+      </c>
+      <c r="L28" t="s">
+        <v>194</v>
+      </c>
+      <c r="M28" t="s">
+        <v>194</v>
+      </c>
+      <c r="N28" t="s">
         <v>171</v>
       </c>
-      <c r="J28" t="s">
+      <c r="O28" t="s">
         <v>18</v>
       </c>
-      <c r="K28">
+      <c r="P28">
         <v>12</v>
       </c>
+      <c r="Q28">
+        <v>8</v>
+      </c>
+      <c r="R28">
+        <v>11</v>
+      </c>
+      <c r="S28" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>172</v>
       </c>
@@ -2473,17 +3088,38 @@
       <c r="H29" t="s">
         <v>90</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
+        <v>194</v>
+      </c>
+      <c r="K29" t="s">
+        <v>194</v>
+      </c>
+      <c r="L29" t="s">
+        <v>194</v>
+      </c>
+      <c r="M29" t="s">
+        <v>194</v>
+      </c>
+      <c r="N29" t="s">
         <v>177</v>
       </c>
-      <c r="J29" t="s">
+      <c r="O29" t="s">
         <v>18</v>
       </c>
-      <c r="K29">
+      <c r="P29">
         <v>12</v>
       </c>
+      <c r="Q29">
+        <v>8</v>
+      </c>
+      <c r="R29">
+        <v>11</v>
+      </c>
+      <c r="S29" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>178</v>
       </c>
@@ -2508,17 +3144,38 @@
       <c r="H30" t="s">
         <v>155</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
+        <v>194</v>
+      </c>
+      <c r="K30" t="s">
+        <v>194</v>
+      </c>
+      <c r="L30" t="s">
+        <v>194</v>
+      </c>
+      <c r="M30" t="s">
+        <v>194</v>
+      </c>
+      <c r="N30" t="s">
         <v>183</v>
       </c>
-      <c r="J30" t="s">
+      <c r="O30" t="s">
         <v>18</v>
       </c>
-      <c r="K30">
+      <c r="P30">
         <v>12</v>
       </c>
+      <c r="Q30">
+        <v>8</v>
+      </c>
+      <c r="R30">
+        <v>11</v>
+      </c>
+      <c r="S30" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>184</v>
       </c>
@@ -2543,14 +3200,35 @@
       <c r="H31" t="s">
         <v>188</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
+        <v>194</v>
+      </c>
+      <c r="K31" t="s">
+        <v>194</v>
+      </c>
+      <c r="L31" t="s">
+        <v>194</v>
+      </c>
+      <c r="M31" t="s">
+        <v>194</v>
+      </c>
+      <c r="N31" t="s">
         <v>189</v>
       </c>
-      <c r="J31" t="s">
+      <c r="O31" t="s">
         <v>18</v>
       </c>
-      <c r="K31">
+      <c r="P31">
         <v>12</v>
+      </c>
+      <c r="Q31">
+        <v>8</v>
+      </c>
+      <c r="R31">
+        <v>11</v>
+      </c>
+      <c r="S31" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>